<commit_message>
152, 200, 681 all possible braces, largest sum subarray
</commit_message>
<xml_diff>
--- a/retro.xlsx
+++ b/retro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chienchichen/Desktop/UQ/course/algorithm/leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A257066E-094D-E14E-8ED1-27ABCB65E510}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AFD7307-DAA1-A848-9486-3537B86934B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="460" windowWidth="28040" windowHeight="15860" xr2:uid="{C1824181-7664-F341-BB4F-E6B34901C6A6}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="48">
   <si>
     <t>Q</t>
   </si>
@@ -142,16 +142,56 @@
   </si>
   <si>
     <t>Unique_Email_Addresses</t>
+  </si>
+  <si>
+    <t>next_closest_time</t>
+  </si>
+  <si>
+    <t>tag</t>
+  </si>
+  <si>
+    <t>dfs</t>
+  </si>
+  <si>
+    <t>Number_of_Islands_mine</t>
+  </si>
+  <si>
+    <t>O(MN)</t>
+  </si>
+  <si>
+    <t>All_possible_braces</t>
+  </si>
+  <si>
+    <t>exponential/O(N)</t>
+  </si>
+  <si>
+    <t>familiarity</t>
+  </si>
+  <si>
+    <t>記Kadane’s algorithm</t>
+  </si>
+  <si>
+    <t>Maximum_Product_Subarray.py</t>
+  </si>
+  <si>
+    <t>看不懂</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -201,13 +241,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -522,10 +564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEB673C5-4A5A-E54D-BB8B-46BFAFC7CF99}">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -534,31 +576,31 @@
     <col min="6" max="6" width="22.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B1" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C1" s="4"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C2" s="3"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -583,8 +625,14 @@
       <c r="H5" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>3</v>
       </c>
@@ -595,7 +643,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>28</v>
       </c>
@@ -606,7 +654,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>395</v>
       </c>
@@ -617,7 +665,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>214</v>
       </c>
@@ -628,7 +676,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>459</v>
       </c>
@@ -639,7 +687,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -650,7 +698,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -661,15 +709,24 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B13" s="6">
+        <v>43820</v>
+      </c>
       <c r="C13" t="s">
         <v>29</v>
       </c>
       <c r="D13" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H13" t="s">
+        <v>45</v>
+      </c>
+      <c r="J13">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -680,7 +737,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -691,7 +748,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -702,7 +759,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -713,7 +770,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>628</v>
       </c>
@@ -727,7 +784,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1</v>
       </c>
@@ -735,7 +792,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>23</v>
       </c>
@@ -746,7 +803,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>904</v>
       </c>
@@ -763,7 +820,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>929</v>
       </c>
@@ -775,6 +832,59 @@
       </c>
       <c r="E22" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>681</v>
+      </c>
+      <c r="B23" s="5">
+        <v>43819</v>
+      </c>
+      <c r="D23" t="s">
+        <v>37</v>
+      </c>
+      <c r="I23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>200</v>
+      </c>
+      <c r="B24" s="5">
+        <v>43820</v>
+      </c>
+      <c r="D24" t="s">
+        <v>40</v>
+      </c>
+      <c r="E24" t="s">
+        <v>41</v>
+      </c>
+      <c r="I24" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B25" s="5">
+        <v>43820</v>
+      </c>
+      <c r="D25" t="s">
+        <v>42</v>
+      </c>
+      <c r="E25" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="7">
+        <v>152</v>
+      </c>
+      <c r="D26" t="s">
+        <v>46</v>
+      </c>
+      <c r="H26" s="7" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>